<commit_message>
came back from backend to root directory still branch arc2
</commit_message>
<xml_diff>
--- a/local_backup.xlsx
+++ b/local_backup.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -719,6 +719,50 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Software Engineering Placement 2025 - (Cloud DevOps)</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Hewlett Packard Enterprise</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Software development methodologies, principles, practices, software development lifecycle, C, C#, C++, Java, Python, Go, Computer architecture, Concurrent programming/multi-threading, Embedded systems, Linux, Networks and communications, Cloud Microservice development, Operating Systems</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Bristol, UK</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2026 Technology (GOTO) Industrial Placement</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>UBS</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Financial Management, Information Technology, Computer Science, Software Engineering, Investment Banking</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>